<commit_message>
Switching back to LDA for a second
</commit_message>
<xml_diff>
--- a/Improvement.xlsx
+++ b/Improvement.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Document" sheetId="1" r:id="rId1"/>
     <sheet name="Titles" sheetId="2" r:id="rId2"/>
+    <sheet name="New Title" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
   <si>
     <t>earn</t>
   </si>
@@ -86,6 +87,15 @@
   </si>
   <si>
     <t xml:space="preserve">weighted </t>
+  </si>
+  <si>
+    <t>money-supply</t>
+  </si>
+  <si>
+    <t>grain-wheat</t>
+  </si>
+  <si>
+    <t>interest-money-fx</t>
   </si>
 </sst>
 </file>
@@ -134,8 +144,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -146,13 +162,19 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -533,11 +555,11 @@
         <v>117</v>
       </c>
       <c r="F2">
-        <f>E2/SUM(E$2:E$11)</f>
+        <f t="shared" ref="F2:F11" si="0">E2/SUM(E$2:E$11)</f>
         <v>4.213179690313288E-2</v>
       </c>
       <c r="G2">
-        <f>(1-D2)*F2</f>
+        <f t="shared" ref="G2:G11" si="1">(1-D2)*F2</f>
         <v>9.2689953186892333E-3</v>
       </c>
     </row>
@@ -558,11 +580,11 @@
         <v>186</v>
       </c>
       <c r="F3">
-        <f>E3/SUM(E$2:E$11)</f>
+        <f t="shared" si="0"/>
         <v>6.697875405113432E-2</v>
       </c>
       <c r="G3">
-        <f>(1-D3)*F3</f>
+        <f t="shared" si="1"/>
         <v>1.674468851278358E-2</v>
       </c>
     </row>
@@ -583,11 +605,11 @@
         <v>87</v>
       </c>
       <c r="F4">
-        <f>E4/SUM(E$2:E$11)</f>
+        <f t="shared" si="0"/>
         <v>3.1328772056175729E-2</v>
       </c>
       <c r="G4">
-        <f>(1-D4)*F4</f>
+        <f t="shared" si="1"/>
         <v>2.0050414115952465E-2</v>
       </c>
     </row>
@@ -608,11 +630,11 @@
         <v>56</v>
       </c>
       <c r="F5">
-        <f>E5/SUM(E$2:E$11)</f>
+        <f t="shared" si="0"/>
         <v>2.0165646380986675E-2</v>
       </c>
       <c r="G5">
-        <f>(1-D5)*F5</f>
+        <f t="shared" si="1"/>
         <v>2.0165646380986675E-2</v>
       </c>
     </row>
@@ -633,11 +655,11 @@
         <v>148</v>
       </c>
       <c r="F6">
-        <f>E6/SUM(E$2:E$11)</f>
+        <f t="shared" si="0"/>
         <v>5.3294922578321934E-2</v>
       </c>
       <c r="G6">
-        <f>(1-D6)*F6</f>
+        <f t="shared" si="1"/>
         <v>2.1317969031328775E-2</v>
       </c>
     </row>
@@ -658,11 +680,11 @@
         <v>180</v>
       </c>
       <c r="F7">
-        <f>E7/SUM(E$2:E$11)</f>
+        <f t="shared" si="0"/>
         <v>6.4818149081742882E-2</v>
       </c>
       <c r="G7">
-        <f>(1-D7)*F7</f>
+        <f t="shared" si="1"/>
         <v>2.2038170687792579E-2</v>
       </c>
     </row>
@@ -683,11 +705,11 @@
         <v>718</v>
       </c>
       <c r="F8">
-        <f>E8/SUM(E$2:E$11)</f>
+        <f t="shared" si="0"/>
         <v>0.25855239467050772</v>
       </c>
       <c r="G8">
-        <f>(1-D8)*F8</f>
+        <f t="shared" si="1"/>
         <v>2.3269715520345687E-2</v>
       </c>
     </row>
@@ -708,11 +730,11 @@
         <v>71</v>
       </c>
       <c r="F9">
-        <f>E9/SUM(E$2:E$11)</f>
+        <f t="shared" si="0"/>
         <v>2.5567158804465251E-2</v>
       </c>
       <c r="G9">
-        <f>(1-D9)*F9</f>
+        <f t="shared" si="1"/>
         <v>2.5567158804465251E-2</v>
       </c>
     </row>
@@ -733,11 +755,11 @@
         <v>133</v>
       </c>
       <c r="F10">
-        <f>E10/SUM(E$2:E$11)</f>
+        <f t="shared" si="0"/>
         <v>4.7893410154843358E-2</v>
       </c>
       <c r="G10">
-        <f>(1-D10)*F10</f>
+        <f t="shared" si="1"/>
         <v>3.1130716600648183E-2</v>
       </c>
     </row>
@@ -758,11 +780,11 @@
         <v>1081</v>
       </c>
       <c r="F11">
-        <f>E11/SUM(E$2:E$11)</f>
+        <f t="shared" si="0"/>
         <v>0.38926899531868925</v>
       </c>
       <c r="G11">
-        <f>(1-D11)*F11</f>
+        <f t="shared" si="1"/>
         <v>3.8926899531868918E-2</v>
       </c>
     </row>
@@ -805,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="H11" sqref="F1:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -854,15 +876,15 @@
         <v>71</v>
       </c>
       <c r="F2">
-        <f>E2/SUM(E$2:E$11)</f>
+        <f t="shared" ref="F2:F11" si="0">E2/SUM(E$2:E$11)</f>
         <v>2.5567158804465251E-2</v>
       </c>
       <c r="G2">
-        <f>D2*F2</f>
+        <f t="shared" ref="G2:G11" si="1">D2*F2</f>
         <v>0</v>
       </c>
       <c r="H2">
-        <f>(1-D2)*F2</f>
+        <f t="shared" ref="H2:H11" si="2">(1-D2)*F2</f>
         <v>2.5567158804465251E-2</v>
       </c>
     </row>
@@ -883,15 +905,15 @@
         <v>718</v>
       </c>
       <c r="F3">
-        <f>E3/SUM(E$2:E$11)</f>
+        <f t="shared" si="0"/>
         <v>0.25855239467050772</v>
       </c>
       <c r="G3">
-        <f>D3*F3</f>
+        <f t="shared" si="1"/>
         <v>0.23528267915016204</v>
       </c>
       <c r="H3">
-        <f>(1-D3)*F3</f>
+        <f t="shared" si="2"/>
         <v>2.3269715520345687E-2</v>
       </c>
     </row>
@@ -912,15 +934,15 @@
         <v>87</v>
       </c>
       <c r="F4">
-        <f>E4/SUM(E$2:E$11)</f>
+        <f t="shared" si="0"/>
         <v>3.1328772056175729E-2</v>
       </c>
       <c r="G4">
-        <f>D4*F4</f>
+        <f t="shared" si="1"/>
         <v>8.7720561757292041E-3</v>
       </c>
       <c r="H4">
-        <f>(1-D4)*F4</f>
+        <f t="shared" si="2"/>
         <v>2.2556715880446523E-2</v>
       </c>
     </row>
@@ -941,15 +963,15 @@
         <v>180</v>
       </c>
       <c r="F5">
-        <f>E5/SUM(E$2:E$11)</f>
+        <f t="shared" si="0"/>
         <v>6.4818149081742882E-2</v>
       </c>
       <c r="G5">
-        <f>D5*F5</f>
+        <f t="shared" si="1"/>
         <v>4.3428159884767732E-2</v>
       </c>
       <c r="H5">
-        <f>(1-D5)*F5</f>
+        <f t="shared" si="2"/>
         <v>2.138998919697515E-2</v>
       </c>
     </row>
@@ -970,15 +992,15 @@
         <v>148</v>
       </c>
       <c r="F6">
-        <f>E6/SUM(E$2:E$11)</f>
+        <f t="shared" si="0"/>
         <v>5.3294922578321934E-2</v>
       </c>
       <c r="G6">
-        <f>D6*F6</f>
+        <f t="shared" si="1"/>
         <v>3.2509902772776378E-2</v>
       </c>
       <c r="H6">
-        <f>(1-D6)*F6</f>
+        <f t="shared" si="2"/>
         <v>2.0785019805545556E-2</v>
       </c>
     </row>
@@ -999,15 +1021,15 @@
         <v>56</v>
       </c>
       <c r="F7">
-        <f>E7/SUM(E$2:E$11)</f>
+        <f t="shared" si="0"/>
         <v>2.0165646380986675E-2</v>
       </c>
       <c r="G7">
-        <f>D7*F7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H7">
-        <f>(1-D7)*F7</f>
+        <f t="shared" si="2"/>
         <v>2.0165646380986675E-2</v>
       </c>
     </row>
@@ -1028,15 +1050,15 @@
         <v>133</v>
       </c>
       <c r="F8">
-        <f>E8/SUM(E$2:E$11)</f>
+        <f t="shared" si="0"/>
         <v>4.7893410154843358E-2</v>
       </c>
       <c r="G8">
-        <f>D8*F8</f>
+        <f t="shared" si="1"/>
         <v>2.8736046092906014E-2</v>
       </c>
       <c r="H8">
-        <f>(1-D8)*F8</f>
+        <f t="shared" si="2"/>
         <v>1.9157364061937344E-2</v>
       </c>
     </row>
@@ -1057,15 +1079,15 @@
         <v>186</v>
       </c>
       <c r="F9">
-        <f>E9/SUM(E$2:E$11)</f>
+        <f t="shared" si="0"/>
         <v>6.697875405113432E-2</v>
       </c>
       <c r="G9">
-        <f>D9*F9</f>
+        <f t="shared" si="1"/>
         <v>5.0903853078862082E-2</v>
       </c>
       <c r="H9">
-        <f>(1-D9)*F9</f>
+        <f t="shared" si="2"/>
         <v>1.6074900972272238E-2</v>
       </c>
     </row>
@@ -1086,15 +1108,15 @@
         <v>117</v>
       </c>
       <c r="F10">
-        <f>E10/SUM(E$2:E$11)</f>
+        <f t="shared" si="0"/>
         <v>4.213179690313288E-2</v>
       </c>
       <c r="G10">
-        <f>D10*F10</f>
+        <f t="shared" si="1"/>
         <v>2.9492257832193013E-2</v>
       </c>
       <c r="H10">
-        <f>(1-D10)*F10</f>
+        <f t="shared" si="2"/>
         <v>1.2639539070939865E-2</v>
       </c>
     </row>
@@ -1115,15 +1137,15 @@
         <v>1081</v>
       </c>
       <c r="F11">
-        <f>E11/SUM(E$2:E$11)</f>
+        <f t="shared" si="0"/>
         <v>0.38926899531868925</v>
       </c>
       <c r="G11">
-        <f>D11*F11</f>
+        <f t="shared" si="1"/>
         <v>0.37759092545912853</v>
       </c>
       <c r="H11">
-        <f>(1-D11)*F11</f>
+        <f t="shared" si="2"/>
         <v>1.1678069859560688E-2</v>
       </c>
     </row>
@@ -1157,4 +1179,329 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="5" width="5.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.97</v>
+      </c>
+      <c r="C2">
+        <v>0.99</v>
+      </c>
+      <c r="D2">
+        <v>0.98</v>
+      </c>
+      <c r="E2">
+        <v>1077</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F11" si="0">E2/SUM(E$2:E$11)</f>
+        <v>0.47340659340659341</v>
+      </c>
+      <c r="G2">
+        <f>D2*F2</f>
+        <v>0.46393846153846152</v>
+      </c>
+      <c r="H2">
+        <f t="shared" ref="H2:H11" si="1">(1-D2)*F2</f>
+        <v>9.4681318681318766E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.67</v>
+      </c>
+      <c r="C3">
+        <v>0.59</v>
+      </c>
+      <c r="D3">
+        <v>0.63</v>
+      </c>
+      <c r="E3">
+        <v>87</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>3.8241758241758239E-2</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G2:G11" si="2">D3*F3</f>
+        <v>2.4092307692307691E-2</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="1"/>
+        <v>1.4149450549450548E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>0.79</v>
+      </c>
+      <c r="C4">
+        <v>0.82</v>
+      </c>
+      <c r="D4">
+        <v>0.81</v>
+      </c>
+      <c r="E4">
+        <v>28</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>1.2307692307692308E-2</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>9.9692307692307702E-3</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>2.338461538461538E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.87</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0.93</v>
+      </c>
+      <c r="E5">
+        <v>76</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>3.340659340659341E-2</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>3.1068131868131874E-2</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>2.3384615384615371E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.95</v>
+      </c>
+      <c r="C6">
+        <v>0.96</v>
+      </c>
+      <c r="D6">
+        <v>0.96</v>
+      </c>
+      <c r="E6">
+        <v>695</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0.30549450549450552</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>0.29327472527472531</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>1.2219780219780232E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>35</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>1.5384615384615385E-2</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>1.5384615384615385E-2</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.78</v>
+      </c>
+      <c r="C8">
+        <v>0.76</v>
+      </c>
+      <c r="D8">
+        <v>0.77</v>
+      </c>
+      <c r="E8">
+        <v>82</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>3.6043956043956042E-2</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>2.7753846153846153E-2</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>8.2901098901098889E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.93</v>
+      </c>
+      <c r="C9">
+        <v>0.86</v>
+      </c>
+      <c r="D9">
+        <v>0.89</v>
+      </c>
+      <c r="E9">
+        <v>119</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>5.2307692307692305E-2</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>4.6553846153846154E-2</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>5.7538461538461528E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>0.34</v>
+      </c>
+      <c r="C10">
+        <v>0.25</v>
+      </c>
+      <c r="D10">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E10">
+        <v>40</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>1.7582417582417582E-2</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>5.0989010989010985E-3</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>1.2483516483516482E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0.96</v>
+      </c>
+      <c r="C11">
+        <v>0.69</v>
+      </c>
+      <c r="D11">
+        <v>0.81</v>
+      </c>
+      <c r="E11">
+        <v>36</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>1.5824175824175824E-2</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>1.2817582417582419E-2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>3.0065934065934058E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>